<commit_message>
EPBDS-2319 generate functions for wrapper types. added slice, sort functions
</commit_message>
<xml_diff>
--- a/DEV/trunk/org.openl.rules/test/rules/helpers/RulesUtilsTest.xlsx
+++ b/DEV/trunk/org.openl.rules/test/rules/helpers/RulesUtilsTest.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="120" windowWidth="24915" windowHeight="12075" activeTab="3"/>
+    <workbookView xWindow="120" yWindow="120" windowWidth="24915" windowHeight="12075" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="byte" sheetId="1" r:id="rId1"/>
@@ -12,7 +12,7 @@
     <sheet name="BigInteger" sheetId="4" r:id="rId3"/>
     <sheet name="BigDecimalValue" sheetId="3" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="125725" refMode="R1C1"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
@@ -52,9 +52,6 @@
     <t>return sum(values);</t>
   </si>
   <si>
-    <t>Method ByteValue testQuaotient(ByteValue number, ByteValue divisor)</t>
-  </si>
-  <si>
     <t>return quaotient(number, divisor);</t>
   </si>
   <si>
@@ -92,6 +89,9 @@
   </si>
   <si>
     <t>return avg(values);</t>
+  </si>
+  <si>
+    <t>Method LongValue testQuaotient(ByteValue number, ByteValue divisor)</t>
   </si>
 </sst>
 </file>
@@ -524,7 +524,7 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B1" s="7"/>
       <c r="C1" s="7"/>
@@ -594,8 +594,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -605,7 +605,7 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B1" s="7"/>
       <c r="C1" s="7"/>
@@ -613,28 +613,28 @@
     </row>
     <row r="10" spans="1:4">
       <c r="B10" s="5" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="C10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="B11" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="B14" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C14" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="15" spans="1:4">
       <c r="B15" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -660,7 +660,7 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B1" s="7"/>
       <c r="C1" s="7"/>
@@ -671,7 +671,7 @@
         <v>9</v>
       </c>
       <c r="D6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -691,8 +691,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -702,7 +702,7 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B1" s="7"/>
       <c r="C1" s="7"/>
@@ -710,15 +710,15 @@
     </row>
     <row r="6" spans="1:5">
       <c r="D6" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="D7" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
EPBDS-2452 rename quotient function
</commit_message>
<xml_diff>
--- a/DEV/trunk/org.openl.rules/test/rules/helpers/RulesUtilsTest.xlsx
+++ b/DEV/trunk/org.openl.rules/test/rules/helpers/RulesUtilsTest.xlsx
@@ -52,9 +52,6 @@
     <t>return sum(values);</t>
   </si>
   <si>
-    <t>return quaotient(number, divisor);</t>
-  </si>
-  <si>
     <t>return min(values);</t>
   </si>
   <si>
@@ -92,6 +89,9 @@
   </si>
   <si>
     <t>Method LongValue testQuaotient(ByteValue number, ByteValue divisor)</t>
+  </si>
+  <si>
+    <t>return quotient(number, divisor);</t>
   </si>
 </sst>
 </file>
@@ -524,7 +524,7 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B1" s="7"/>
       <c r="C1" s="7"/>
@@ -595,7 +595,7 @@
   <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -605,7 +605,7 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B1" s="7"/>
       <c r="C1" s="7"/>
@@ -613,28 +613,28 @@
     </row>
     <row r="10" spans="1:4">
       <c r="B10" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="B11" s="4" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="B14" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C14" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="15" spans="1:4">
       <c r="B15" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -660,7 +660,7 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B1" s="7"/>
       <c r="C1" s="7"/>
@@ -671,7 +671,7 @@
         <v>9</v>
       </c>
       <c r="D6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -702,7 +702,7 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B1" s="7"/>
       <c r="C1" s="7"/>
@@ -710,15 +710,15 @@
     </row>
     <row r="6" spans="1:5">
       <c r="D6" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="D7" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
EPBDS-2364 rename or to anyTrue
</commit_message>
<xml_diff>
--- a/DEV/trunk/org.openl.rules/test/rules/helpers/RulesUtilsTest.xlsx
+++ b/DEV/trunk/org.openl.rules/test/rules/helpers/RulesUtilsTest.xlsx
@@ -4,20 +4,21 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="120" windowWidth="24915" windowHeight="12075" activeTab="1"/>
+    <workbookView xWindow="120" yWindow="120" windowWidth="24915" windowHeight="12075" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="byte" sheetId="1" r:id="rId1"/>
     <sheet name="ByteValue" sheetId="2" r:id="rId2"/>
     <sheet name="BigInteger" sheetId="4" r:id="rId3"/>
     <sheet name="BigDecimalValue" sheetId="3" r:id="rId4"/>
+    <sheet name="logical functions" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>C1</t>
   </si>
@@ -92,6 +93,12 @@
   </si>
   <si>
     <t>return quotient(number, divisor);</t>
+  </si>
+  <si>
+    <t>Method boolean checkOr()</t>
+  </si>
+  <si>
+    <t>return anyTrue(new boolean[]{true, false});</t>
   </si>
 </sst>
 </file>
@@ -594,7 +601,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
@@ -727,4 +734,32 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="C7:C8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="3" max="3" width="34.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="7" spans="3:3">
+      <c r="C7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="3:3">
+      <c r="C8" t="s">
+        <v>26</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Add Unit-tests. Comment testFirstDayOfQurter and testLastDayOfQurter. Fix containsAll(T[] container, T[] testArray).
</commit_message>
<xml_diff>
--- a/DEV/trunk/org.openl.rules/test/rules/helpers/RulesUtilsTest.xlsx
+++ b/DEV/trunk/org.openl.rules/test/rules/helpers/RulesUtilsTest.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="601" uniqueCount="259">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="609" uniqueCount="267">
   <si>
     <t>C1</t>
   </si>
@@ -808,6 +808,30 @@
   </si>
   <si>
     <t>Method Date testFirstDayOfQuarter(int date1)</t>
+  </si>
+  <si>
+    <t>Method Date testLastDayOfQuarter(int date1)</t>
+  </si>
+  <si>
+    <t>return lastDateOfQuarter(date1);</t>
+  </si>
+  <si>
+    <t>return lastDayOfMonth(date1);</t>
+  </si>
+  <si>
+    <t>Method int testLastDayOfMonth(Date date1)</t>
+  </si>
+  <si>
+    <t>Method int testGetMonth(Date date1)</t>
+  </si>
+  <si>
+    <t>return month(date1);</t>
+  </si>
+  <si>
+    <t>Method int testMonthDiff(Date date1, Date date2)</t>
+  </si>
+  <si>
+    <t>return monthDiff(date1, date2);</t>
   </si>
 </sst>
 </file>
@@ -2808,10 +2832,10 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:B18"/>
+  <dimension ref="B2:B30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2877,6 +2901,46 @@
     <row r="18" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B18" s="11" t="s">
         <v>257</v>
+      </c>
+    </row>
+    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B20" s="10" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="21" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B21" s="11" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="23" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B23" s="10" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="24" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B24" s="11" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="26" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B26" s="10" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="27" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B27" s="11" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="29" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B29" s="10" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="30" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B30" s="11" t="s">
+        <v>266</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Finish RulesutilsClass unit-tests. Update jUnit to 4.11
</commit_message>
<xml_diff>
--- a/DEV/trunk/org.openl.rules/test/rules/helpers/RulesUtilsTest.xlsx
+++ b/DEV/trunk/org.openl.rules/test/rules/helpers/RulesUtilsTest.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="12" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="600" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView activeTab="22" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="600" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
     <sheet name="MaxMinTests" sheetId="1" state="visible" r:id="rId2"/>
@@ -24,14 +24,20 @@
     <sheet name="Product" sheetId="14" state="visible" r:id="rId15"/>
     <sheet name="Logical" sheetId="15" state="visible" r:id="rId16"/>
     <sheet name="Round" sheetId="16" state="visible" r:id="rId17"/>
-    <sheet name="Sheet17" sheetId="17" state="visible" r:id="rId18"/>
+    <sheet name="MaxMinTests2" sheetId="17" state="visible" r:id="rId18"/>
+    <sheet name="Add" sheetId="18" state="visible" r:id="rId19"/>
+    <sheet name="AddAll" sheetId="19" state="visible" r:id="rId20"/>
+    <sheet name="Remove" sheetId="20" state="visible" r:id="rId21"/>
+    <sheet name="Empty" sheetId="21" state="visible" r:id="rId22"/>
+    <sheet name="Sheet22" sheetId="22" state="visible" r:id="rId23"/>
+    <sheet name="small and big" sheetId="23" state="visible" r:id="rId24"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="719" uniqueCount="351">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="957" uniqueCount="495">
   <si>
     <t>Tests to test rules helper methods for Max and Min value of different types</t>
   </si>
@@ -978,6 +984,24 @@
     <t>Method float testFloatCopySign(float x, float y)</t>
   </si>
   <si>
+    <t>Method double testCos(double x)</t>
+  </si>
+  <si>
+    <t>return cos(x);</t>
+  </si>
+  <si>
+    <t>Method double testToDegrees(double x)</t>
+  </si>
+  <si>
+    <t>return toDegrees(x);</t>
+  </si>
+  <si>
+    <t>Method double testToRadians(double x)</t>
+  </si>
+  <si>
+    <t>return toRadians(x);</t>
+  </si>
+  <si>
     <t>Method double testByteTypeProduct(byte[] inputArray)</t>
   </si>
   <si>
@@ -1084,6 +1108,420 @@
   </si>
   <si>
     <t>Method BigDecimal testBigDecimalScaleRoundRoundMethod(BigDecimal num, int scale, int roundMethod)</t>
+  </si>
+  <si>
+    <t>Method int testIntegerTypeMax(int x, int y)</t>
+  </si>
+  <si>
+    <t>Method int testIntegerTypeMin(int x, int y)</t>
+  </si>
+  <si>
+    <t>return max(x, y);</t>
+  </si>
+  <si>
+    <t>return min(x, y);</t>
+  </si>
+  <si>
+    <t>Method double testDoubleTypeMax(double x, double y)</t>
+  </si>
+  <si>
+    <t>Method double testDoubleTypeMin(double x, double y)</t>
+  </si>
+  <si>
+    <t>Method float testFloatTypeMax(float x, float y)</t>
+  </si>
+  <si>
+    <t>Method float testFloatTypeMin(float x, float y)</t>
+  </si>
+  <si>
+    <t>Method long testLongTypeMax(long x, long y)</t>
+  </si>
+  <si>
+    <t>Method long testLongTypeMin(long x, long y)</t>
+  </si>
+  <si>
+    <t>Method Integer testIntegerMax(Integer x, Integer y)</t>
+  </si>
+  <si>
+    <t>Method Integer testIntegerMin(Integer x, Integer y)</t>
+  </si>
+  <si>
+    <t>Method Double testDoubleMax(Double x, Double y)</t>
+  </si>
+  <si>
+    <t>Method Double testDoubleMin(Double x, Double y)</t>
+  </si>
+  <si>
+    <t>Method Float testFloatMax(Float x, Float y)</t>
+  </si>
+  <si>
+    <t>Method Float testFloatMin(Float x, Float y)</t>
+  </si>
+  <si>
+    <t>Method Long testLongMax(Long x, Long y)</t>
+  </si>
+  <si>
+    <t>Method Long testLongMin(Long x, Long y)</t>
+  </si>
+  <si>
+    <t>Method BigInteger testBigIntegerMax(BigInteger x, BigInteger y)</t>
+  </si>
+  <si>
+    <t>Method BigInteger testBigIntegerMin(BigInteger x, BigInteger y)</t>
+  </si>
+  <si>
+    <t>Method BigDecimal testBigDecimalMax(BigDecimal x, BigDecimal y)</t>
+  </si>
+  <si>
+    <t>Method BigDecimal testBigDecimalMin(BigDecimal x, BigDecimal y)</t>
+  </si>
+  <si>
+    <t>Method boolean[] testBooleanTypeAdd(boolean[] inArr, boolean el)</t>
+  </si>
+  <si>
+    <t>Method short[] testShortTypeAdd(short[] inArr, short el)</t>
+  </si>
+  <si>
+    <t>return add(inArr, el);</t>
+  </si>
+  <si>
+    <t>Method boolean[] testBooleanTypeAdd(boolean[] inArr, int pos, boolean el)</t>
+  </si>
+  <si>
+    <t>Method short[] testShortTypeAdd(short[] inArr, int pos, short el)</t>
+  </si>
+  <si>
+    <t>return add(inArr, pos, el);</t>
+  </si>
+  <si>
+    <t>Method byte[] testByteTypeAdd(byte[] inArr, byte el)</t>
+  </si>
+  <si>
+    <t>Method Object[] testObjectTypeAddIgnoreNulls(Object[] inArr, ObjectValue el)</t>
+  </si>
+  <si>
+    <t>return addIgnoreNull(inArr, el);</t>
+  </si>
+  <si>
+    <t>Method byte[] testByteTypeAdd(byte[] inArr, int pos, byte el)</t>
+  </si>
+  <si>
+    <t>Method Object[] testObjectTypeAddIgnoreNulls(Object[] inArr, int pos, ObjectValue el)</t>
+  </si>
+  <si>
+    <t>return addIgnoreNull(inArr, pos, el);</t>
+  </si>
+  <si>
+    <t>Method char[] testCharTypeAdd(char[] inArr, char el)</t>
+  </si>
+  <si>
+    <t>Method char[] testCharTypeAdd(char[] inArr, int pos, char el)</t>
+  </si>
+  <si>
+    <t>Method double[] testDoubleTypeAdd(double[] inArr, double el)</t>
+  </si>
+  <si>
+    <t>Method double[] testDoubleTypeAdd(double[] inArr, int pos, double el)</t>
+  </si>
+  <si>
+    <t>Method float[] testFloatTypeAdd(float[] inArr, float el)</t>
+  </si>
+  <si>
+    <t>Method float[] testFloatTypeAdd(float[] inArr, int pos, float el)</t>
+  </si>
+  <si>
+    <t>Method int[] testIntegerTypeAdd(int[] inArr, int el)</t>
+  </si>
+  <si>
+    <t>Method int[] testIntegerTypeAdd(int[] inArr, int pos, int el)</t>
+  </si>
+  <si>
+    <t>Method long[] testLongTypeAdd(long[] inArr, long el)</t>
+  </si>
+  <si>
+    <t>Method long[] testLongTypeAdd(long[] inArr, int pos, long el)</t>
+  </si>
+  <si>
+    <t>Method Object[] testObjectTypeAdd(Object[] inArr, ObjectValue el)</t>
+  </si>
+  <si>
+    <t>Method Object[] testObjectTypeAdd(Object[] inArr, int pos, ObjectValue el)</t>
+  </si>
+  <si>
+    <t>Method byte[] testByteTypeAddAll(byte[] inArr1, byte[] inArr2)</t>
+  </si>
+  <si>
+    <t>return addAll(inArr1, inArr2);</t>
+  </si>
+  <si>
+    <t>Method char[] testCharTypeAddAll(char[] inArr1, char[] inArr2)</t>
+  </si>
+  <si>
+    <t>Method double[] testDoubleTypeAddAll(double[] inArr1, double[] inArr2)</t>
+  </si>
+  <si>
+    <t>Method float[] testFloatTypeAddAll(float[] inArr1, float[] inArr2)</t>
+  </si>
+  <si>
+    <t>Method int[] testIntegerTypeAddAll(int[] inArr1, int[] inArr2)</t>
+  </si>
+  <si>
+    <t>Method long[] testLongTypeAddAll(long[] inArr1, long[] inArr2)</t>
+  </si>
+  <si>
+    <t>Method Object[] testObjectAddAll(Object[] inArr1, Object[] inArr2)</t>
+  </si>
+  <si>
+    <t>Method short[] testShortTypeAddAll(short[] inArr1, short[] inArr2)</t>
+  </si>
+  <si>
+    <t>Method boolean[] testBooleanTypeAddAll(boolean[] inArr1, boolean[] inArr2)</t>
+  </si>
+  <si>
+    <t>Method boolean[] testBooleanTypeRemove(boolean[] inArr,int pos)</t>
+  </si>
+  <si>
+    <t>Method boolean[] testBooleanTypeRemoveElement(boolean[] inArr,boolean el)</t>
+  </si>
+  <si>
+    <t>return remove(inArr, pos);</t>
+  </si>
+  <si>
+    <t>return removeElement(inArr, el);</t>
+  </si>
+  <si>
+    <t>Method byte[] testByteTypeRemove(byte[] inArr,int pos)</t>
+  </si>
+  <si>
+    <t>Method byte[] testByteTypeRemoveElement(byte[] inArr, byte el)</t>
+  </si>
+  <si>
+    <t>Method char[] testCharTypeRemove(char[] inArr,int pos)</t>
+  </si>
+  <si>
+    <t>Method char[] testCharTypeRemoveElement(char[] inArr, char el)</t>
+  </si>
+  <si>
+    <t>Method double[] testDoubleTypeRemove(double[] inArr,int pos)</t>
+  </si>
+  <si>
+    <t>Method double[] testDoubleTypeRemoveElement(double[] inArr, double el)</t>
+  </si>
+  <si>
+    <t>Method float[] testFloatTypeRemove(float[] inArr,int pos)</t>
+  </si>
+  <si>
+    <t>Method float[] testFloatTypeRemoveElement(float[] inArr, float el)</t>
+  </si>
+  <si>
+    <t>Method int[] testIntegerTypeRemove(int[] inArr,int pos)</t>
+  </si>
+  <si>
+    <t>Method int[] testIntegerTypeRemoveElement(int[] inArr, int el)</t>
+  </si>
+  <si>
+    <t>Method long[] testLongTypeRemove(long[] inArr,int pos)</t>
+  </si>
+  <si>
+    <t>Method long[] testLongTypeRemoveElement(long[] inArr, long el)</t>
+  </si>
+  <si>
+    <t>Method Object[] testObjectTypeRemove(Object[] inArr,int pos)</t>
+  </si>
+  <si>
+    <t>Method Object[] testObjectTypeRemoveElement(Object[] inArr, Object el)</t>
+  </si>
+  <si>
+    <t>Method short[] testShortTypeRemove(short[] inArr,int pos)</t>
+  </si>
+  <si>
+    <t>Method short[] testShortTypeRemoveElement(short[] inArr, short el)</t>
+  </si>
+  <si>
+    <t>Method boolean testObjectIsEmpty(Object[] inArr)</t>
+  </si>
+  <si>
+    <t>return isEmpty(inArr);</t>
+  </si>
+  <si>
+    <t>Method boolean testByteTypeIsEmpty(byte[] inArr)</t>
+  </si>
+  <si>
+    <t>Method boolean testCharTypeIsEmpty(char[] inArr)</t>
+  </si>
+  <si>
+    <t>Method boolean testShortTypeIsEmpty(short[] inArr)</t>
+  </si>
+  <si>
+    <t>Method boolean testIntegerTypeIsEmpty(int[] inArr)</t>
+  </si>
+  <si>
+    <t>Method boolean testLongTypeIsEmpty(long[] inArr)</t>
+  </si>
+  <si>
+    <t>Method boolean testFloatTypeIsEmpty(float[] inArr)</t>
+  </si>
+  <si>
+    <t>Method boolean testDateIsEmpty(Date[] inArr)</t>
+  </si>
+  <si>
+    <t>Method boolean testBigDecimalIsEmpty(BigDecimal[] inArr)</t>
+  </si>
+  <si>
+    <t>Method boolean testBigIntegerIsEmpty(BigInteger[] inArr)</t>
+  </si>
+  <si>
+    <t>Method boolean testStringIsEmpty(String[] inArr)</t>
+  </si>
+  <si>
+    <t>Method boolean testStartsWith(String str, String prefix)</t>
+  </si>
+  <si>
+    <t>return startsWith(str, prefix);</t>
+  </si>
+  <si>
+    <t>Method String testSubString(String str, int startIndex)</t>
+  </si>
+  <si>
+    <t>return substring(str, startIndex);</t>
+  </si>
+  <si>
+    <t>Method boolean testEndsWith(String str, String prefix)</t>
+  </si>
+  <si>
+    <t>return endsWith(str, prefix);</t>
+  </si>
+  <si>
+    <t>Method String testSubString(String str, int startIndex, int endIndex)</t>
+  </si>
+  <si>
+    <t>return substring(str, startIndex, endindex);</t>
+  </si>
+  <si>
+    <t>Method String testRemoveStart(String str, String prefix)</t>
+  </si>
+  <si>
+    <t>return removeStart(str, prefix);</t>
+  </si>
+  <si>
+    <t>Method String testRemoveEnd(String str, String prefix)</t>
+  </si>
+  <si>
+    <t>return removeEnd(str, prefix);</t>
+  </si>
+  <si>
+    <t>Method String testUpperCase(String str)</t>
+  </si>
+  <si>
+    <t>return upperCase(str);</t>
+  </si>
+  <si>
+    <t>Method String testLowerCase(String str)</t>
+  </si>
+  <si>
+    <t>return lowerCase(str);</t>
+  </si>
+  <si>
+    <t>Method String testReplace(String str, String whatReplace, String onReplace)</t>
+  </si>
+  <si>
+    <t>return replace(str, whatReplace, onReplace);</t>
+  </si>
+  <si>
+    <t>Method String testReplace(String str, String whatReplace, String onReplace, int replaceCount)</t>
+  </si>
+  <si>
+    <t>return replace(str, whatReplace, onReplace, replaceCount);</t>
+  </si>
+  <si>
+    <t>Method byte testByteTypeSmall(byte[] inArray, int pos)</t>
+  </si>
+  <si>
+    <t>Method byte testByteTypeBig(byte[] inArray, int pos)</t>
+  </si>
+  <si>
+    <t>return small(inArray, pos);</t>
+  </si>
+  <si>
+    <t>return big(inArray, pos);</t>
+  </si>
+  <si>
+    <t>Method short testShortTypeSmall(short[] inArray, int pos)</t>
+  </si>
+  <si>
+    <t>Method short testShortTypeBig(short[] inArray, int pos)</t>
+  </si>
+  <si>
+    <t>Method int testIntegerTypeSmall(int[] inArray, int pos)</t>
+  </si>
+  <si>
+    <t>Method int testIntegerTypeBig(int[] inArray, int pos)</t>
+  </si>
+  <si>
+    <t>Method long testLongTypeSmall(long[] inArray, int pos)</t>
+  </si>
+  <si>
+    <t>Method long testLongTypeBig(long[] inArray, int pos)</t>
+  </si>
+  <si>
+    <t>Method float testFloatTypeSmall(float[] inArray, int pos)</t>
+  </si>
+  <si>
+    <t>Method float testFloatTypeBig(float[] inArray, int pos)</t>
+  </si>
+  <si>
+    <t>Method double testDoubleTypeSmall(double[] inArray, int pos)</t>
+  </si>
+  <si>
+    <t>Method double testDoubleTypeBig(double[] inArray, int pos)</t>
+  </si>
+  <si>
+    <t>Method BigDecimal testBigDecimalSmall(BigDecimal[] inArray, int pos)</t>
+  </si>
+  <si>
+    <t>Method BigDecimal testBigDecimalBig(BigDecimal[] inArray, int pos)</t>
+  </si>
+  <si>
+    <t>Method BigInteger testBigIntegerSmall(BigInteger[] inArray, int pos)</t>
+  </si>
+  <si>
+    <t>Method BigInteger testBigIntegerBig(BigInteger[] inArray, int pos)</t>
+  </si>
+  <si>
+    <t>Method Byte testByteSmall(Byte[] inArray, int pos)</t>
+  </si>
+  <si>
+    <t>Method Byte testByteBig(Byte[] inArray, int pos)</t>
+  </si>
+  <si>
+    <t>Method Short testShortSmall(Short[] inArray, int pos)</t>
+  </si>
+  <si>
+    <t>Method Short testShortBig(Short[] inArray, int pos)</t>
+  </si>
+  <si>
+    <t>Method Integer testIntegerSmall(Integer[] inArray, int pos)</t>
+  </si>
+  <si>
+    <t>Method Integer testIntegerBig(Integer[] inArray, int pos)</t>
+  </si>
+  <si>
+    <t>Method Long testLongSmall(Long[] inArray, int pos)</t>
+  </si>
+  <si>
+    <t>Method Long testLongBig(Long[] inArray, int pos)</t>
+  </si>
+  <si>
+    <t>Method Float testFloatSmall(Float[] inArray, int pos)</t>
+  </si>
+  <si>
+    <t>Method Float testFloatBig(Float[] inArray, int pos)</t>
+  </si>
+  <si>
+    <t>Method Double testDoubleSmall(Double[] inArray, int pos)</t>
+  </si>
+  <si>
+    <t>Method Double testDoubleBig(Double[] inArray, int pos)</t>
   </si>
 </sst>
 </file>
@@ -1394,8 +1832,8 @@
   </sheetPr>
   <dimension ref="A1:I114"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="133" zoomScaleNormal="133" zoomScalePageLayoutView="100">
-      <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="B4" activeCellId="0" pane="topLeft" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2645,7 +3083,7 @@
   </sheetPr>
   <dimension ref="A1:E25"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="133" zoomScaleNormal="133" zoomScalePageLayoutView="100">
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
       <selection activeCell="C28" activeCellId="0" pane="topLeft" sqref="C28"/>
     </sheetView>
   </sheetViews>
@@ -2787,7 +3225,7 @@
   </sheetPr>
   <dimension ref="A1:F28"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="133" zoomScaleNormal="133" zoomScalePageLayoutView="100">
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
       <selection activeCell="F21" activeCellId="0" pane="topLeft" sqref="F21"/>
     </sheetView>
   </sheetViews>
@@ -2945,7 +3383,7 @@
   </sheetPr>
   <dimension ref="C7:C8"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="133" zoomScaleNormal="133" zoomScalePageLayoutView="100">
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
       <selection activeCell="C8" activeCellId="0" pane="topLeft" sqref="C8"/>
     </sheetView>
   </sheetViews>
@@ -2982,10 +3420,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B2:B108"/>
+  <dimension ref="B2:B117"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A82" view="normal" windowProtection="false" workbookViewId="0" zoomScale="133" zoomScaleNormal="133" zoomScalePageLayoutView="100">
-      <selection activeCell="B108" activeCellId="0" pane="topLeft" sqref="B108"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A91" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="B118" activeCellId="0" pane="topLeft" sqref="B118"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3419,6 +3857,36 @@
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="108">
       <c r="B108" s="13" t="s">
         <v>313</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="110">
+      <c r="B110" s="12" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="111">
+      <c r="B111" s="13" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="113">
+      <c r="B113" s="12" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="114">
+      <c r="B114" s="13" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="116">
+      <c r="B116" s="12" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="117">
+      <c r="B117" s="13" t="s">
+        <v>320</v>
       </c>
     </row>
   </sheetData>
@@ -3439,7 +3907,7 @@
   </sheetPr>
   <dimension ref="B2:D27"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="133" zoomScaleNormal="133" zoomScalePageLayoutView="100">
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
       <selection activeCell="B2" activeCellId="0" pane="topLeft" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -3454,20 +3922,20 @@
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="2">
       <c r="B2" s="12" t="s">
-        <v>315</v>
+        <v>321</v>
       </c>
       <c r="C2" s="15"/>
       <c r="D2" s="12" t="s">
-        <v>316</v>
+        <v>322</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="3">
       <c r="B3" s="13" t="s">
-        <v>317</v>
+        <v>323</v>
       </c>
       <c r="C3" s="15"/>
       <c r="D3" s="13" t="s">
-        <v>317</v>
+        <v>323</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="4">
@@ -3477,20 +3945,20 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="5">
       <c r="B5" s="12" t="s">
-        <v>318</v>
+        <v>324</v>
       </c>
       <c r="C5" s="15"/>
       <c r="D5" s="12" t="s">
-        <v>319</v>
+        <v>325</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="6">
       <c r="B6" s="13" t="s">
-        <v>317</v>
+        <v>323</v>
       </c>
       <c r="C6" s="15"/>
       <c r="D6" s="13" t="s">
-        <v>317</v>
+        <v>323</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="7">
@@ -3500,20 +3968,20 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="8">
       <c r="B8" s="12" t="s">
-        <v>320</v>
+        <v>326</v>
       </c>
       <c r="C8" s="15"/>
       <c r="D8" s="12" t="s">
-        <v>321</v>
+        <v>327</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="9">
       <c r="B9" s="13" t="s">
-        <v>317</v>
+        <v>323</v>
       </c>
       <c r="C9" s="15"/>
       <c r="D9" s="13" t="s">
-        <v>317</v>
+        <v>323</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="10">
@@ -3523,20 +3991,20 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="11">
       <c r="B11" s="12" t="s">
-        <v>322</v>
+        <v>328</v>
       </c>
       <c r="C11" s="15"/>
       <c r="D11" s="12" t="s">
-        <v>323</v>
+        <v>329</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="12">
       <c r="B12" s="13" t="s">
-        <v>317</v>
+        <v>323</v>
       </c>
       <c r="C12" s="15"/>
       <c r="D12" s="13" t="s">
-        <v>317</v>
+        <v>323</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="13">
@@ -3546,20 +4014,20 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="14">
       <c r="B14" s="12" t="s">
-        <v>324</v>
+        <v>330</v>
       </c>
       <c r="C14" s="15"/>
       <c r="D14" s="12" t="s">
-        <v>325</v>
+        <v>331</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="15">
       <c r="B15" s="13" t="s">
-        <v>317</v>
+        <v>323</v>
       </c>
       <c r="C15" s="15"/>
       <c r="D15" s="13" t="s">
-        <v>317</v>
+        <v>323</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="16">
@@ -3569,20 +4037,20 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="17">
       <c r="B17" s="12" t="s">
-        <v>326</v>
+        <v>332</v>
       </c>
       <c r="C17" s="15"/>
       <c r="D17" s="12" t="s">
-        <v>327</v>
+        <v>333</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="18">
       <c r="B18" s="13" t="s">
-        <v>317</v>
+        <v>323</v>
       </c>
       <c r="C18" s="15"/>
       <c r="D18" s="13" t="s">
-        <v>317</v>
+        <v>323</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="19">
@@ -3593,13 +4061,13 @@
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="20">
       <c r="C20" s="15"/>
       <c r="D20" s="12" t="s">
-        <v>328</v>
+        <v>334</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="21">
       <c r="C21" s="15"/>
       <c r="D21" s="13" t="s">
-        <v>317</v>
+        <v>323</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="22">
@@ -3609,13 +4077,13 @@
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="23">
       <c r="C23" s="15"/>
       <c r="D23" s="12" t="s">
-        <v>329</v>
+        <v>335</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="24">
       <c r="C24" s="15"/>
       <c r="D24" s="13" t="s">
-        <v>317</v>
+        <v>323</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="27"/>
@@ -3650,62 +4118,62 @@
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="3">
       <c r="B3" s="12" t="s">
-        <v>330</v>
+        <v>336</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="4">
       <c r="B4" s="13" t="s">
-        <v>331</v>
+        <v>337</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="6">
       <c r="B6" s="12" t="s">
-        <v>332</v>
+        <v>338</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="7">
       <c r="B7" s="13" t="s">
-        <v>331</v>
+        <v>337</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="9">
       <c r="B9" s="12" t="s">
-        <v>333</v>
+        <v>339</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="10">
       <c r="B10" s="13" t="s">
-        <v>334</v>
+        <v>340</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="12">
       <c r="B12" s="12" t="s">
-        <v>335</v>
+        <v>341</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="13">
       <c r="B13" s="13" t="s">
-        <v>334</v>
+        <v>340</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="15">
       <c r="B15" s="12" t="s">
-        <v>336</v>
+        <v>342</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="16">
       <c r="B16" s="13" t="s">
-        <v>337</v>
+        <v>343</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="18">
       <c r="B18" s="12" t="s">
-        <v>338</v>
+        <v>344</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="19">
       <c r="B19" s="13" t="s">
-        <v>337</v>
+        <v>343</v>
       </c>
     </row>
   </sheetData>
@@ -3739,92 +4207,92 @@
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="3">
       <c r="B3" s="12" t="s">
-        <v>339</v>
+        <v>345</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="4">
       <c r="B4" s="13" t="s">
-        <v>340</v>
+        <v>346</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="6">
       <c r="B6" s="12" t="s">
-        <v>341</v>
+        <v>347</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="7">
       <c r="B7" s="13" t="s">
-        <v>340</v>
+        <v>346</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="9">
       <c r="B9" s="12" t="s">
-        <v>342</v>
+        <v>348</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="10">
       <c r="B10" s="13" t="s">
-        <v>343</v>
+        <v>349</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="12">
       <c r="B12" s="12" t="s">
-        <v>344</v>
+        <v>350</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="13">
       <c r="B13" s="13" t="s">
-        <v>343</v>
+        <v>349</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="15">
       <c r="B15" s="12" t="s">
-        <v>345</v>
+        <v>351</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="16">
       <c r="B16" s="13" t="s">
-        <v>346</v>
+        <v>352</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="18">
       <c r="B18" s="12" t="s">
-        <v>347</v>
+        <v>353</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="19">
       <c r="B19" s="13" t="s">
-        <v>346</v>
+        <v>352</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="21">
       <c r="B21" s="12" t="s">
-        <v>348</v>
+        <v>354</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="22">
       <c r="B22" s="13" t="s">
-        <v>340</v>
+        <v>346</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="24">
       <c r="B24" s="12" t="s">
-        <v>349</v>
+        <v>355</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="25">
       <c r="B25" s="13" t="s">
-        <v>343</v>
+        <v>349</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="27">
       <c r="B27" s="12" t="s">
-        <v>350</v>
+        <v>356</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="28">
       <c r="B28" s="13" t="s">
-        <v>346</v>
+        <v>352</v>
       </c>
     </row>
   </sheetData>
@@ -3843,17 +4311,528 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1"/>
+  <dimension ref="B3:D31"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
+      <selection activeCell="B30" activeCellId="0" pane="topLeft" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="50.2704081632653"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="56.4540816326531"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="11.5204081632653"/>
   </cols>
-  <sheetData/>
+  <sheetData>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="3">
+      <c r="B3" s="12" t="s">
+        <v>357</v>
+      </c>
+      <c r="D3" s="12" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="4">
+      <c r="B4" s="13" t="s">
+        <v>359</v>
+      </c>
+      <c r="D4" s="13" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="5"/>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="6">
+      <c r="B6" s="12" t="s">
+        <v>361</v>
+      </c>
+      <c r="D6" s="12" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="7">
+      <c r="B7" s="13" t="s">
+        <v>359</v>
+      </c>
+      <c r="D7" s="13" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="8"/>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="9">
+      <c r="B9" s="12" t="s">
+        <v>363</v>
+      </c>
+      <c r="D9" s="12" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="10">
+      <c r="B10" s="13" t="s">
+        <v>359</v>
+      </c>
+      <c r="D10" s="13" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="11"/>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="12">
+      <c r="B12" s="12" t="s">
+        <v>365</v>
+      </c>
+      <c r="D12" s="12" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="13">
+      <c r="B13" s="13" t="s">
+        <v>359</v>
+      </c>
+      <c r="D13" s="13" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="14"/>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="15">
+      <c r="B15" s="12" t="s">
+        <v>367</v>
+      </c>
+      <c r="D15" s="12" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="16">
+      <c r="B16" s="13" t="s">
+        <v>359</v>
+      </c>
+      <c r="D16" s="13" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="17"/>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="18">
+      <c r="B18" s="12" t="s">
+        <v>369</v>
+      </c>
+      <c r="D18" s="12" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="19">
+      <c r="B19" s="13" t="s">
+        <v>359</v>
+      </c>
+      <c r="D19" s="13" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="20"/>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="21">
+      <c r="B21" s="12" t="s">
+        <v>371</v>
+      </c>
+      <c r="D21" s="12" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="22">
+      <c r="B22" s="13" t="s">
+        <v>359</v>
+      </c>
+      <c r="D22" s="13" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="23"/>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="24">
+      <c r="B24" s="12" t="s">
+        <v>373</v>
+      </c>
+      <c r="D24" s="12" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="25">
+      <c r="B25" s="13" t="s">
+        <v>359</v>
+      </c>
+      <c r="D25" s="13" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="26"/>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="27">
+      <c r="B27" s="12" t="s">
+        <v>375</v>
+      </c>
+      <c r="D27" s="12" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="28">
+      <c r="B28" s="13" t="s">
+        <v>359</v>
+      </c>
+      <c r="D28" s="13" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="29"/>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="30">
+      <c r="B30" s="12" t="s">
+        <v>377</v>
+      </c>
+      <c r="D30" s="12" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="31">
+      <c r="B31" s="13" t="s">
+        <v>359</v>
+      </c>
+      <c r="D31" s="13" t="s">
+        <v>360</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="B1:D48"/>
+  <sheetViews>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="B2" activeCellId="0" pane="topLeft" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.3"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="70.1683673469388"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="68.015306122449"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="11.5204081632653"/>
+  </cols>
+  <sheetData>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1"/>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="2">
+      <c r="B2" s="12" t="s">
+        <v>379</v>
+      </c>
+      <c r="D2" s="12" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="3">
+      <c r="B3" s="13" t="s">
+        <v>381</v>
+      </c>
+      <c r="D3" s="13" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="5">
+      <c r="B5" s="12" t="s">
+        <v>382</v>
+      </c>
+      <c r="D5" s="12" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="6">
+      <c r="B6" s="13" t="s">
+        <v>384</v>
+      </c>
+      <c r="D6" s="13" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="7"/>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="8">
+      <c r="B8" s="12" t="s">
+        <v>385</v>
+      </c>
+      <c r="D8" s="12" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="9">
+      <c r="B9" s="13" t="s">
+        <v>381</v>
+      </c>
+      <c r="D9" s="13" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="11">
+      <c r="B11" s="12" t="s">
+        <v>388</v>
+      </c>
+      <c r="D11" s="12" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="12">
+      <c r="B12" s="13" t="s">
+        <v>384</v>
+      </c>
+      <c r="D12" s="13" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="14">
+      <c r="B14" s="12" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="15">
+      <c r="B15" s="13" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="17">
+      <c r="B17" s="12" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="18">
+      <c r="B18" s="13" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="20">
+      <c r="B20" s="12" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="21">
+      <c r="B21" s="13" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="23">
+      <c r="B23" s="12" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="24">
+      <c r="B24" s="13" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="26">
+      <c r="B26" s="12" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="27">
+      <c r="B27" s="13" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="29">
+      <c r="B29" s="12" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="30">
+      <c r="B30" s="13" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="32">
+      <c r="B32" s="12" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="33">
+      <c r="B33" s="13" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="35">
+      <c r="B35" s="12" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="36">
+      <c r="B36" s="13" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="38">
+      <c r="B38" s="12" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="39">
+      <c r="B39" s="13" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="41">
+      <c r="B41" s="12" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="42">
+      <c r="B42" s="13" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="44">
+      <c r="B44" s="12" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="45">
+      <c r="B45" s="13" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="47">
+      <c r="B47" s="12" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="48">
+      <c r="B48" s="13" t="s">
+        <v>384</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="B2:B27"/>
+  <sheetViews>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="B27" activeCellId="0" pane="topLeft" sqref="B27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="56.4540816326531"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="11.5204081632653"/>
+  </cols>
+  <sheetData>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="2">
+      <c r="B2" s="12" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="3">
+      <c r="B3" s="13" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="4"/>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="5">
+      <c r="B5" s="12" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="6">
+      <c r="B6" s="13" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="8">
+      <c r="B8" s="12" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="9">
+      <c r="B9" s="13" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="11">
+      <c r="B11" s="12" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="12">
+      <c r="B12" s="13" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="14">
+      <c r="B14" s="12" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="15">
+      <c r="B15" s="13" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="17">
+      <c r="B17" s="12" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="18">
+      <c r="B18" s="13" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="20">
+      <c r="B20" s="12" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="21">
+      <c r="B21" s="13" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="23">
+      <c r="B23" s="12" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="24">
+      <c r="B24" s="13" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="26">
+      <c r="B26" s="12" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="27">
+      <c r="B27" s="13" t="s">
+        <v>404</v>
+      </c>
+    </row>
+  </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
@@ -3871,7 +4850,7 @@
   </sheetPr>
   <dimension ref="A1:E45"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="133" zoomScaleNormal="133" zoomScalePageLayoutView="100">
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
       <selection activeCell="C4" activeCellId="0" pane="topLeft" sqref="C4"/>
     </sheetView>
   </sheetViews>
@@ -4098,6 +5077,715 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="B2:D27"/>
+  <sheetViews>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="B2" activeCellId="0" pane="topLeft" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="53.4948979591837"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="57.5357142857143"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="11.5204081632653"/>
+  </cols>
+  <sheetData>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="2">
+      <c r="B2" s="12" t="s">
+        <v>413</v>
+      </c>
+      <c r="D2" s="12" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="3">
+      <c r="B3" s="13" t="s">
+        <v>415</v>
+      </c>
+      <c r="D3" s="13" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="5">
+      <c r="B5" s="12" t="s">
+        <v>417</v>
+      </c>
+      <c r="D5" s="12" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="6">
+      <c r="B6" s="13" t="s">
+        <v>415</v>
+      </c>
+      <c r="D6" s="13" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="8">
+      <c r="B8" s="12" t="s">
+        <v>419</v>
+      </c>
+      <c r="D8" s="12" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="9">
+      <c r="B9" s="13" t="s">
+        <v>415</v>
+      </c>
+      <c r="D9" s="13" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="11">
+      <c r="B11" s="12" t="s">
+        <v>421</v>
+      </c>
+      <c r="D11" s="12" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="12">
+      <c r="B12" s="13" t="s">
+        <v>415</v>
+      </c>
+      <c r="D12" s="13" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="14">
+      <c r="B14" s="12" t="s">
+        <v>423</v>
+      </c>
+      <c r="D14" s="12" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="15">
+      <c r="B15" s="13" t="s">
+        <v>415</v>
+      </c>
+      <c r="D15" s="13" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="17">
+      <c r="B17" s="12" t="s">
+        <v>425</v>
+      </c>
+      <c r="D17" s="12" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="18">
+      <c r="B18" s="13" t="s">
+        <v>415</v>
+      </c>
+      <c r="D18" s="13" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="20">
+      <c r="B20" s="12" t="s">
+        <v>427</v>
+      </c>
+      <c r="D20" s="12" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="21">
+      <c r="B21" s="13" t="s">
+        <v>415</v>
+      </c>
+      <c r="D21" s="13" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="23">
+      <c r="B23" s="12" t="s">
+        <v>429</v>
+      </c>
+      <c r="D23" s="12" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="24">
+      <c r="B24" s="13" t="s">
+        <v>415</v>
+      </c>
+      <c r="D24" s="13" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="26">
+      <c r="B26" s="12" t="s">
+        <v>431</v>
+      </c>
+      <c r="D26" s="12" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="27">
+      <c r="B27" s="13" t="s">
+        <v>415</v>
+      </c>
+      <c r="D27" s="13" t="s">
+        <v>416</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="B2:B33"/>
+  <sheetViews>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="B2" activeCellId="0" pane="topLeft" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="62.2295918367347"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="11.5204081632653"/>
+  </cols>
+  <sheetData>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="2">
+      <c r="B2" s="12" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="3">
+      <c r="B3" s="13" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="5">
+      <c r="B5" s="12" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="6">
+      <c r="B6" s="13" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="8">
+      <c r="B8" s="12" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="9">
+      <c r="B9" s="13" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="11">
+      <c r="B11" s="12" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="12">
+      <c r="B12" s="13" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="14">
+      <c r="B14" s="12" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="15">
+      <c r="B15" s="13" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="17">
+      <c r="B17" s="12" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="18">
+      <c r="B18" s="13" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="20">
+      <c r="B20" s="12" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="21">
+      <c r="B21" s="13" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="23">
+      <c r="B23" s="12" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="24">
+      <c r="B24" s="13" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="26">
+      <c r="B26" s="12" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="27">
+      <c r="B27" s="13" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="29">
+      <c r="B29" s="12" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="30">
+      <c r="B30" s="13" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="32">
+      <c r="B32" s="12" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="33">
+      <c r="B33" s="13" t="s">
+        <v>434</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="B1:B31"/>
+  <sheetViews>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="B2" activeCellId="0" pane="topLeft" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.3"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="78.9081632653061"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="11.5204081632653"/>
+  </cols>
+  <sheetData>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1"/>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="2">
+      <c r="B2" s="12" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="3">
+      <c r="B3" s="13" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="4"/>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="5">
+      <c r="B5" s="12" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="6">
+      <c r="B6" s="13" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="7"/>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="8">
+      <c r="B8" s="12" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="9">
+      <c r="B9" s="13" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="10"/>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="11">
+      <c r="B11" s="12" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="12">
+      <c r="B12" s="13" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="13"/>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="14">
+      <c r="B14" s="12" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="15">
+      <c r="B15" s="13" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="16"/>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="17">
+      <c r="B17" s="12" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="18">
+      <c r="B18" s="13" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="19"/>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="20">
+      <c r="B20" s="12" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="21">
+      <c r="B21" s="13" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="22"/>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="23">
+      <c r="B23" s="12" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="24">
+      <c r="B24" s="13" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="25"/>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="26">
+      <c r="B26" s="12" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="27">
+      <c r="B27" s="13" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="28"/>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="29">
+      <c r="B29" s="12" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="30">
+      <c r="B30" s="13" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="31"/>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="B2:D42"/>
+  <sheetViews>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="D20" activeCellId="0" pane="topLeft" sqref="D20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="50"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="65.4642857142857"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="11.5204081632653"/>
+  </cols>
+  <sheetData>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="2">
+      <c r="B2" s="12" t="s">
+        <v>465</v>
+      </c>
+      <c r="D2" s="12" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="3">
+      <c r="B3" s="13" t="s">
+        <v>467</v>
+      </c>
+      <c r="D3" s="13" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="5">
+      <c r="B5" s="12" t="s">
+        <v>469</v>
+      </c>
+      <c r="D5" s="12" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="6">
+      <c r="B6" s="13" t="s">
+        <v>467</v>
+      </c>
+      <c r="D6" s="13" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="8">
+      <c r="B8" s="12" t="s">
+        <v>471</v>
+      </c>
+      <c r="D8" s="12" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="9">
+      <c r="B9" s="13" t="s">
+        <v>467</v>
+      </c>
+      <c r="D9" s="13" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="11">
+      <c r="B11" s="12" t="s">
+        <v>473</v>
+      </c>
+      <c r="D11" s="12" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="12">
+      <c r="B12" s="13" t="s">
+        <v>467</v>
+      </c>
+      <c r="D12" s="13" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="14">
+      <c r="B14" s="12" t="s">
+        <v>475</v>
+      </c>
+      <c r="D14" s="12" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="15">
+      <c r="B15" s="13" t="s">
+        <v>467</v>
+      </c>
+      <c r="D15" s="13" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="17">
+      <c r="B17" s="12" t="s">
+        <v>477</v>
+      </c>
+      <c r="D17" s="12" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="18">
+      <c r="B18" s="13" t="s">
+        <v>467</v>
+      </c>
+      <c r="D18" s="13" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="20">
+      <c r="B20" s="12" t="s">
+        <v>479</v>
+      </c>
+      <c r="D20" s="12" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="21">
+      <c r="B21" s="13" t="s">
+        <v>467</v>
+      </c>
+      <c r="D21" s="13" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="23">
+      <c r="B23" s="12" t="s">
+        <v>481</v>
+      </c>
+      <c r="D23" s="12" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="24">
+      <c r="B24" s="13" t="s">
+        <v>467</v>
+      </c>
+      <c r="D24" s="13" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="26">
+      <c r="B26" s="12" t="s">
+        <v>483</v>
+      </c>
+      <c r="D26" s="12" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="27">
+      <c r="B27" s="13" t="s">
+        <v>467</v>
+      </c>
+      <c r="D27" s="13" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="29">
+      <c r="B29" s="12" t="s">
+        <v>485</v>
+      </c>
+      <c r="D29" s="12" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="30">
+      <c r="B30" s="13" t="s">
+        <v>467</v>
+      </c>
+      <c r="D30" s="13" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="32">
+      <c r="B32" s="12" t="s">
+        <v>487</v>
+      </c>
+      <c r="D32" s="12" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="33">
+      <c r="B33" s="13" t="s">
+        <v>467</v>
+      </c>
+      <c r="D33" s="13" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="35">
+      <c r="B35" s="12" t="s">
+        <v>489</v>
+      </c>
+      <c r="D35" s="12" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="36">
+      <c r="B36" s="13" t="s">
+        <v>467</v>
+      </c>
+      <c r="D36" s="13" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="38">
+      <c r="B38" s="12" t="s">
+        <v>491</v>
+      </c>
+      <c r="D38" s="12" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="39">
+      <c r="B39" s="13" t="s">
+        <v>467</v>
+      </c>
+      <c r="D39" s="13" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="41">
+      <c r="B41" s="12" t="s">
+        <v>493</v>
+      </c>
+      <c r="D41" s="12" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="42">
+      <c r="B42" s="13" t="s">
+        <v>467</v>
+      </c>
+      <c r="D42" s="13" t="s">
+        <v>468</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
@@ -4105,7 +5793,7 @@
   </sheetPr>
   <dimension ref="A1:E50"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="133" zoomScaleNormal="133" zoomScalePageLayoutView="100">
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
       <selection activeCell="C4" activeCellId="0" pane="topLeft" sqref="C4"/>
     </sheetView>
   </sheetViews>
@@ -4380,7 +6068,7 @@
   </sheetPr>
   <dimension ref="A1:E52"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="133" zoomScaleNormal="133" zoomScalePageLayoutView="100">
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
       <selection activeCell="C4" activeCellId="0" pane="topLeft" sqref="C4"/>
     </sheetView>
   </sheetViews>
@@ -4643,8 +6331,8 @@
   </sheetPr>
   <dimension ref="A1:E28"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="B1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="133" zoomScaleNormal="133" zoomScalePageLayoutView="100">
-      <selection activeCell="E3" activeCellId="0" pane="topLeft" sqref="E3"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="D12" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="E28" activeCellId="0" pane="topLeft" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4830,7 +6518,7 @@
   </sheetPr>
   <dimension ref="A1:D28"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="133" zoomScaleNormal="133" zoomScalePageLayoutView="100">
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
       <selection activeCell="C3" activeCellId="0" pane="topLeft" sqref="C3"/>
     </sheetView>
   </sheetViews>
@@ -4961,7 +6649,7 @@
   </sheetPr>
   <dimension ref="B3:B4"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="133" zoomScaleNormal="133" zoomScalePageLayoutView="100">
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
       <selection activeCell="B3" activeCellId="0" pane="topLeft" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -5000,7 +6688,7 @@
   </sheetPr>
   <dimension ref="B3:D7"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="133" zoomScaleNormal="133" zoomScalePageLayoutView="100">
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
       <selection activeCell="B3" activeCellId="0" pane="topLeft" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -5063,7 +6751,7 @@
   </sheetPr>
   <dimension ref="A1:D37"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="133" zoomScaleNormal="133" zoomScalePageLayoutView="100">
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
       <selection activeCell="B36" activeCellId="0" pane="topLeft" sqref="B36"/>
     </sheetView>
   </sheetViews>

</xml_diff>